<commit_message>
Update bug list status
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List-201505.xlsx
+++ b/Docs/Testing Issue List-201505.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -1346,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,9 +1758,13 @@
       <c r="C20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="18">
+        <v>42135</v>
+      </c>
       <c r="G20" s="15" t="s">
         <v>12</v>
       </c>
@@ -2215,7 +2219,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>